<commit_message>
Fikset oppførsel ved negativt forbruk ++
</commit_message>
<xml_diff>
--- a/Prissatser_nettleie_BKK.xlsx
+++ b/Prissatser_nettleie_BKK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asmund.fossum\Documents\Strompriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B192E07-A9F4-4A2A-B546-8F519A316FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7599C26F-5625-4AA2-AD3E-0EF816F661C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-120" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{846E382B-0241-4CBD-8E39-0843AEB05BE3}"/>
+    <workbookView xWindow="-27468" yWindow="2340" windowWidth="23040" windowHeight="12120" xr2:uid="{846E382B-0241-4CBD-8E39-0843AEB05BE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Privatkunde" sheetId="1" r:id="rId1"/>
@@ -309,13 +309,13 @@
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711BC047-462D-4916-A1EB-232D01805D89}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,7 +785,7 @@
         <v>0.01</v>
       </c>
       <c r="H4" s="2">
-        <v>0.01</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF15A06-53F4-4CEC-A80E-4A8322FD1FCA}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1268,7 +1268,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="11">
@@ -1280,12 +1280,12 @@
       <c r="D2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="16">
         <v>45575</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="7">
         <f>B2/12</f>
         <v>950</v>
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="11">
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="7">
         <v>70</v>
       </c>
@@ -1346,7 +1346,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="9">
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="9">
         <v>58</v>
       </c>

</xml_diff>